<commit_message>
removed old files + general update
</commit_message>
<xml_diff>
--- a/.Study plan/MasterDegree_StudyPlan.xlsx
+++ b/.Study plan/MasterDegree_StudyPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\GitHub\Repo\UniPD-MSc-Computer-Science-courses\.Study plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE12ECD-820C-4045-B897-C147B07F733A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F1DF86-605E-48AD-8251-D9D9ED4170D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CCEDFCE-005C-40C2-92E8-4E076261F21E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>Computability</t>
   </si>
@@ -212,9 +212,6 @@
   </si>
   <si>
     <t>Cyber physical systems and IoT security</t>
-  </si>
-  <si>
-    <t>5/6 credits awarded</t>
   </si>
   <si>
     <r>
@@ -242,6 +239,9 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>4/6 credits awarded (waiting for last 2 CFU)</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -523,9 +523,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -556,8 +553,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1349,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B725-BD0D-4291-9550-3225AF05D5FC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1369,36 +1372,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="A1" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1425,7 +1428,7 @@
       <c r="H4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="24"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -1452,7 +1455,7 @@
       <c r="H5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="25"/>
+      <c r="J5" s="24"/>
     </row>
     <row r="6" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
@@ -1480,7 +1483,7 @@
         <v>28</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="25"/>
+      <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
@@ -1507,7 +1510,7 @@
       <c r="H7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="19"/>
+      <c r="J7" s="18"/>
       <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1697,28 +1700,28 @@
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="7">
         <v>2</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="7">
         <v>1</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="7">
         <v>6</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="11" t="s">
         <v>28</v>
       </c>
       <c r="J15" s="16"/>
@@ -1751,79 +1754,81 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:9" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="27">
+        <v>2</v>
+      </c>
+      <c r="F17" s="27">
+        <v>1</v>
+      </c>
+      <c r="G17" s="27">
+        <v>6</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D18" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E18" s="20">
         <v>2</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F18" s="20">
         <v>1</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G18" s="20">
         <v>6</v>
       </c>
-      <c r="H17" s="22"/>
-    </row>
-    <row r="18" spans="1:9" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="21">
+      <c r="H18" s="21"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="21">
-        <v>1</v>
-      </c>
-      <c r="G18" s="21">
+      <c r="D19" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="20">
+        <v>2</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="20">
         <v>6</v>
       </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="21">
-        <v>2</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="21">
-        <v>6</v>
-      </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="18" t="s">
-        <v>55</v>
+      <c r="H19" s="21"/>
+      <c r="I19" s="30" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>